<commit_message>
adding cases for 02_clean transform. So far, focusing on the production variables. Still to talk about value of production
</commit_message>
<xml_diff>
--- a/config/pam_unit_conversions.xlsx
+++ b/config/pam_unit_conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\projetos\pesquisa_agricola_municipal\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17AB3C3-95BB-427A-A3F1-D6A73B4BD1EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C1590-A897-4C41-9F7E-0488CBE9A9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{7951A0C4-0C4F-4A58-9209-806B597D6F71}"/>
+    <workbookView xWindow="645" yWindow="2025" windowWidth="12405" windowHeight="15285" xr2:uid="{7951A0C4-0C4F-4A58-9209-806B597D6F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="37">
   <si>
     <t>produto</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>coco_da_bahia</t>
+  </si>
+  <si>
+    <t>grao</t>
+  </si>
+  <si>
+    <t>coco</t>
   </si>
 </sst>
 </file>
@@ -514,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097507A2-A6A4-4D3C-BB95-6EF286E11ECD}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,10 +1500,10 @@
         <v>2001</v>
       </c>
       <c r="D34" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1523,10 +1529,10 @@
         <v>9999</v>
       </c>
       <c r="D35" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F35">
         <v>1</v>

</xml_diff>

<commit_message>
added alternative unit cases for production in 02_clean...
</commit_message>
<xml_diff>
--- a/config/pam_unit_conversions.xlsx
+++ b/config/pam_unit_conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\projetos\pesquisa_agricola_municipal\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C1590-A897-4C41-9F7E-0488CBE9A9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B635F570-B1F0-4472-A0E9-080E38B67ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="2025" windowWidth="12405" windowHeight="15285" xr2:uid="{7951A0C4-0C4F-4A58-9209-806B597D6F71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{7951A0C4-0C4F-4A58-9209-806B597D6F71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -140,13 +140,13 @@
     <t>mil_cachos</t>
   </si>
   <si>
-    <t>coco_da_bahia</t>
-  </si>
-  <si>
     <t>grao</t>
   </si>
   <si>
     <t>coco</t>
+  </si>
+  <si>
+    <t>coco_da_baia</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,10 +1500,10 @@
         <v>2001</v>
       </c>
       <c r="D34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -1529,10 +1529,10 @@
         <v>9999</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>1974</v>

</xml_diff>